<commit_message>
Duck shoot changes to electronics design
</commit_message>
<xml_diff>
--- a/Design/Chassis Design/SpeedTestCalculations.xlsx
+++ b/Design/Chassis Design/SpeedTestCalculations.xlsx
@@ -64,7 +64,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -134,7 +134,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
@@ -420,7 +420,7 @@
   <dimension ref="B2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>130</v>
+        <v>270</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -492,7 +492,7 @@
       </c>
       <c r="C7" s="4">
         <f>C2/60</f>
-        <v>2.1666666666666665</v>
+        <v>4.5</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
@@ -504,7 +504,7 @@
       </c>
       <c r="C8" s="3">
         <f>C6/C7</f>
-        <v>16.499376348934952</v>
+        <v>7.9441441680057165</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>

</xml_diff>